<commit_message>
pdf viewer con HTML5
</commit_message>
<xml_diff>
--- a/dev_docs/hercules/estimacion y entregas.xlsx
+++ b/dev_docs/hercules/estimacion y entregas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <r>
       <t>Proyecto</t>
@@ -113,12 +113,27 @@
   <si>
     <t>Hacer una lista de control de accesos basada en roles (seguridad por roles no por usuario)</t>
   </si>
+  <si>
+    <t>Crear catálogo de usuarios</t>
+  </si>
+  <si>
+    <t>Agregar busqueda por nombre, nick y email</t>
+  </si>
+  <si>
+    <t>Como dueño del negocio, quiero ver los reportes de ventas del día, de días anteriores y comparativas, en tiempo real y en ambiente web, para tomar decisiones oportunas sin importar donde me encuentre.</t>
+  </si>
+  <si>
+    <t>Crear página reportes</t>
+  </si>
+  <si>
+    <t>crear pdf de prueba(incluyendo filtros y visualizacion en un tab del sistema)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +193,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FFA6A6A6"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF808080"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -214,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -245,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +611,7 @@
       </c>
       <c r="C5">
         <f>SUM(B10:B100)</f>
-        <v>6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -672,12 +696,57 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>